<commit_message>
RESOLVIENDO EJERCICIOS: Formulas , Operadores , Referencia de Celdas Mixta(Columnas - Filas) - Absolutas - Relativas
</commit_message>
<xml_diff>
--- a/NivelBasico/Módulo 4 - Operadores.xlsx
+++ b/NivelBasico/Módulo 4 - Operadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\db\Nik Denilson\Cursos\EXCEL\NivelBasico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C23E67A-67F1-44D7-892B-F7EF707354DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B933F415-5207-4BC8-892C-FB2A5CEABB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="854" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2897,7 +2897,7 @@
     <cellStyle name="Normal 5" xfId="20" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="Porcentual 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3003,29 +3003,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -11762,10 +11742,10 @@
     <mergeCell ref="E20:F20"/>
   </mergeCells>
   <conditionalFormatting sqref="I16 K26 K28 K30 I45">
-    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="VERDADERO">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="VERDADERO">
       <formula>NOT(ISERROR(SEARCH("VERDADERO",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="FALSO">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="FALSO">
       <formula>NOT(ISERROR(SEARCH("FALSO",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12493,12 +12473,12 @@
     <mergeCell ref="E20:F20"/>
   </mergeCells>
   <conditionalFormatting sqref="I16 K26 K28 K30 I45">
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="VERDADERO">
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="VERDADERO">
       <formula>NOT(ISERROR(SEARCH("VERDADERO",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45 K30 K28 K26 I16">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="FALSO">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="FALSO">
       <formula>NOT(ISERROR(SEARCH("FALSO",I16)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>